<commit_message>
Finished the presentation examples and added screenshot method to base
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/POM_GoogleSearchTestData.xlsx
+++ b/src/test/resources/TestData/POM_GoogleSearchTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15225" windowHeight="3510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12780" windowHeight="2340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Incorta</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Search Data</t>
   </si>
   <si>
-    <t>Incorta: The Fastest Way to Analyze Complex Business Data</t>
-  </si>
-  <si>
     <t>Texts</t>
   </si>
   <si>
@@ -40,22 +34,16 @@
     <t>Firefox</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t>TEAM</t>
-  </si>
-  <si>
-    <t>ABOUT</t>
-  </si>
-  <si>
-    <t>Menu Item</t>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>What is Selenium? Introduction to Selenium Automation Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,6 +84,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -144,7 +135,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +170,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,54 +382,42 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>